<commit_message>
agrego datos del producto bruto interno per capita
</commit_message>
<xml_diff>
--- a/model/model.xlsx
+++ b/model/model.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Graphics" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Graphics" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -21,54 +20,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t xml:space="preserve">Año</t>
+    <t>Año</t>
   </si>
   <si>
-    <t xml:space="preserve">Tráfico entrante (min)</t>
+    <t>Tráfico entrante (min)</t>
   </si>
   <si>
-    <t xml:space="preserve">Tráfico saliente (min)</t>
+    <t>Tráfico saliente (min)</t>
   </si>
   <si>
-    <t xml:space="preserve">Número Teléfonos</t>
+    <t>Número Teléfonos</t>
   </si>
   <si>
-    <t xml:space="preserve">Localidades Beneficiadas</t>
+    <t>Localidades Beneficiadas</t>
   </si>
   <si>
-    <t xml:space="preserve">Lineas Móviles</t>
+    <t>Lineas Móviles</t>
   </si>
   <si>
-    <t xml:space="preserve">Tráfico móvil entrante</t>
+    <t>Tráfico móvil entrante</t>
   </si>
   <si>
-    <t xml:space="preserve">Tráfico móvil saliente</t>
+    <t>Tráfico móvil saliente</t>
   </si>
   <si>
-    <t xml:space="preserve">MMS originados</t>
+    <t>MMS originados</t>
   </si>
   <si>
-    <t xml:space="preserve">SMS originados</t>
+    <t>SMS originados</t>
   </si>
   <si>
-    <t xml:space="preserve">Población Rural</t>
+    <t>Población Rural</t>
   </si>
   <si>
-    <t xml:space="preserve">Producto Bruto Interno</t>
+    <t>Producto Bruto Interno</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="###.00E+00;[RED]\-###.00E+00"/>
-    <numFmt numFmtId="166" formatCode="##0.00E+00;[RED]\-##0.00E+00"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -76,41 +73,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,7 +89,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -130,53 +97,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -235,15 +170,30 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -252,12 +202,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Tráfico rural entrante vs Número de telefonos por año</a:t>
@@ -265,10 +215,12 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -287,9 +239,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
@@ -310,30 +259,32 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="faa61a"/>
+                  <a:srgbClr val="FAA61A"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Data!$B$2:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>140968904</c:v>
+                  <c:v> </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>127374052</c:v>
@@ -365,8 +316,8 @@
                 <c:pt idx="10">
                   <c:v>14231412</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -412,11 +363,19 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="8953822"/>
-        <c:axId val="35083725"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="143092544"/>
+        <c:axId val="159150016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="8953822"/>
+        <c:axId val="143092544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -429,12 +388,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tráfico entrante (min)</a:t>
@@ -442,6 +401,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -451,7 +411,7 @@
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -460,18 +420,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35083725"/>
+        <c:crossAx val="159150016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35083725"/>
+        <c:axId val="159150016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -481,7 +442,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
+                <a:srgbClr val="B3B3B3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -493,12 +454,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Número de telefonos</a:t>
@@ -506,6 +467,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -515,7 +477,7 @@
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -524,13 +486,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8953822"/>
+        <c:crossAx val="143092544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -538,13 +501,14 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
+            <a:srgbClr val="B3B3B3"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -557,31 +521,40 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+            <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -590,12 +563,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Tráfico rural saliente vs Número de teléfonos por año</a:t>
@@ -603,10 +576,12 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -625,9 +600,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
@@ -648,21 +620,24 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="faa61a"/>
+                  <a:srgbClr val="FAA61A"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -750,11 +725,19 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="78757444"/>
-        <c:axId val="65188351"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="143097152"/>
+        <c:axId val="154233664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="78757444"/>
+        <c:axId val="143097152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,12 +750,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tráfico rural saliente (min)</a:t>
@@ -780,6 +763,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -789,7 +773,7 @@
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -798,18 +782,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65188351"/>
+        <c:crossAx val="154233664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65188351"/>
+        <c:axId val="154233664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,7 +804,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
+                <a:srgbClr val="B3B3B3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -831,12 +816,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Número de teléfonos</a:t>
@@ -844,6 +829,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -853,7 +839,7 @@
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -862,13 +848,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78757444"/>
+        <c:crossAx val="143097152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -876,13 +863,14 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
+            <a:srgbClr val="B3B3B3"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -895,31 +883,40 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+            <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -928,12 +925,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Tráfico rural entrante vs Localidades Beneficiadas (anual)</a:t>
@@ -941,10 +938,12 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -963,9 +962,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
@@ -986,30 +982,32 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="faa61a"/>
+                  <a:srgbClr val="FAA61A"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Data!$B$2:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>140968904</c:v>
+                  <c:v> </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>127374052</c:v>
@@ -1041,8 +1039,8 @@
                 <c:pt idx="10">
                   <c:v>14231412</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -1088,11 +1086,19 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="54050064"/>
-        <c:axId val="13823151"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="159214400"/>
+        <c:axId val="137666560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54050064"/>
+        <c:axId val="159214400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1105,12 +1111,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tráfico rural entrante (min)</a:t>
@@ -1118,6 +1124,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1127,7 +1134,7 @@
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -1136,18 +1143,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13823151"/>
+        <c:crossAx val="137666560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="13823151"/>
+        <c:axId val="137666560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1157,7 +1165,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
+                <a:srgbClr val="B3B3B3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -1169,12 +1177,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Localidades Beneficiadas</a:t>
@@ -1182,6 +1190,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1191,7 +1200,7 @@
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -1200,13 +1209,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54050064"/>
+        <c:crossAx val="159214400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1214,13 +1224,14 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
+            <a:srgbClr val="B3B3B3"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1233,31 +1244,40 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+            <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1266,12 +1286,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Líneas móviles vs Trafico rural entrante (anual)</a:t>
@@ -1279,10 +1299,12 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1301,9 +1323,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
@@ -1324,30 +1343,32 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="faa61a"/>
+                  <a:srgbClr val="FAA61A"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Data!$B$2:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>140968904</c:v>
+                  <c:v> </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>127374052</c:v>
@@ -1379,8 +1400,8 @@
                 <c:pt idx="10">
                   <c:v>14231412</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -1426,11 +1447,19 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="54829050"/>
-        <c:axId val="43820333"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="137668288"/>
+        <c:axId val="137668864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54829050"/>
+        <c:axId val="137668288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1443,12 +1472,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Trafico rural entrante (min)</a:t>
@@ -1456,16 +1485,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="###.00E+00;[RED]\-###.00E+00" sourceLinked="0"/>
+        <c:numFmt formatCode="###.00E+00;[Red]\-###.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -1474,18 +1504,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43820333"/>
+        <c:crossAx val="137668864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43820333"/>
+        <c:axId val="137668864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1495,7 +1526,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
+                <a:srgbClr val="B3B3B3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -1507,12 +1538,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Líneas móviles</a:t>
@@ -1520,16 +1551,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="###.00E+00;[RED]\-###.00E+00" sourceLinked="0"/>
+        <c:numFmt formatCode="###.00E+00;[Red]\-###.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -1538,13 +1570,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54829050"/>
+        <c:crossAx val="137668288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1552,13 +1585,14 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
+            <a:srgbClr val="B3B3B3"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1571,31 +1605,40 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+            <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1604,12 +1647,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Tráfico rural entrante vs saliente anual, periodo 2006 al 2016</a:t>
@@ -1621,6 +1664,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1639,9 +1683,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:noFill/>
             </a:ln>
@@ -1662,30 +1703,31 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:trendline>
             <c:spPr>
               <a:ln>
                 <a:solidFill>
-                  <a:srgbClr val="faa61a"/>
+                  <a:srgbClr val="FAA61A"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>Data!$B$2:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>140968904</c:v>
+                  <c:v> </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>127374052</c:v>
@@ -1717,8 +1759,8 @@
                 <c:pt idx="10">
                   <c:v>14231412</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -1764,11 +1806,19 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="27300909"/>
-        <c:axId val="92609672"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="137670592"/>
+        <c:axId val="137671168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27300909"/>
+        <c:axId val="137670592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1781,12 +1831,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Trafico entrante (min)</a:t>
@@ -1796,14 +1846,14 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="###.00E+00;[RED]\-###.00E+00" sourceLinked="0"/>
+        <c:numFmt formatCode="###.00E+00;[Red]\-###.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -1812,18 +1862,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92609672"/>
+        <c:crossAx val="137671168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92609672"/>
+        <c:axId val="137671168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1833,7 +1884,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
+                <a:srgbClr val="B3B3B3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -1845,12 +1896,12 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Trafico saliente (min)</a:t>
@@ -1860,14 +1911,14 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="##0.00E+00;[RED]\-##0.00E+00" sourceLinked="0"/>
+        <c:numFmt formatCode="##0.00E+00;[Red]\-##0.00E+00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -1876,13 +1927,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27300909"/>
+        <c:crossAx val="137670592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1890,7 +1942,7 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
+            <a:srgbClr val="B3B3B3"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
@@ -1909,29 +1961,36 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+            <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
               <a:latin typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1945,14 +2004,14 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>161280</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvPr id="2" name="1 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1680120" y="2257560"/>
-        <a:ext cx="6095160" cy="3430440"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1975,14 +2034,14 @@
       <xdr:row>57</xdr:row>
       <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvPr id="3" name="2 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="891000" y="5997960"/>
-        <a:ext cx="6098040" cy="3293280"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2005,14 +2064,14 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvPr id="4" name="3 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7576200" y="2320200"/>
-        <a:ext cx="6263640" cy="3522600"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2035,14 +2094,14 @@
       <xdr:row>56</xdr:row>
       <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvPr id="5" name="4 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7675920" y="5920200"/>
-        <a:ext cx="5847120" cy="3239280"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2056,7 +2115,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -2070,14 +2129,14 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>136800</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvPr id="4" name="3 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="812880" y="162720"/>
-        <a:ext cx="7634520" cy="4037760"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2090,35 +2149,317 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.38"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="13" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2156,429 +2497,428 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>2006</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>140968904</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
         <v>182470409</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2">
         <v>14221</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>9191</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>55606894</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2">
         <v>1211904425</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2">
         <v>4300811363</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2">
         <v>9549167</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2">
         <v>797061621</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2">
         <v>6869817</v>
       </c>
-      <c r="L2" s="0" t="n">
-        <v>88643193061.748</v>
+      <c r="L2">
+        <v>88643193061.748001</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2007</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3">
         <v>127374052</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>181013062</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3">
         <v>14780</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>9198</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>89562518</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3">
         <v>1376440097</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3">
         <v>8250368519</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3">
         <v>12831376</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3">
         <v>3209720669</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3">
         <v>6845990</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3">
         <v>102170981144.136</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>2008</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4">
         <v>96895035</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>139257563</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4">
         <v>17868</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4">
         <v>9521</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4">
         <v>116677743</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4">
         <v>1736104032</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4">
         <v>12515102774</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4">
         <v>18530696</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4">
         <v>3878812329</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4">
         <v>6859181</v>
       </c>
-      <c r="L4" s="0" t="n">
-        <v>120550599815.441</v>
+      <c r="L4">
+        <v>120550599815.44099</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>2009</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>74342629</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>105819960</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5">
         <v>16419</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>9494</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>132173951</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5">
         <v>2141368661</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5">
         <v>17377847673</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5">
         <v>16819258</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5">
         <v>3661910890</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5">
         <v>6890468</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5">
         <v>120822986521.479</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>2010</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6">
         <v>56613331</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6">
         <v>89226667</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6">
         <v>21340</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6">
         <v>12635</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6">
         <v>150419094</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6">
         <v>2694342886</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6">
         <v>19648912176</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6">
         <v>18916421</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6">
         <v>4358109394</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6">
         <v>6923368</v>
       </c>
-      <c r="L6" s="0" t="n">
-        <v>147528937028.778</v>
+      <c r="L6">
+        <v>147528937028.77802</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>2011</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>34965133</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7">
         <v>60372566</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7">
         <v>21782</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>12671</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>166611829</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7">
         <v>3803911316</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7">
         <v>26756356826</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7">
         <v>20024700</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7">
         <v>5428075569</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7">
         <v>6958778</v>
       </c>
-      <c r="L7" s="0" t="n">
-        <v>171761737046.585</v>
+      <c r="L7">
+        <v>171761737046.58499</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>2012</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8">
         <v>28968553</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>51726115</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8">
         <v>20999</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8">
         <v>13250</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8">
         <v>117377681</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8">
         <v>4212811737</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8">
         <v>32613594433</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8">
         <v>19597174</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8">
         <v>7860995193</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8">
         <v>6995674</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8">
         <v>192648999090.082</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>2013</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9">
         <v>23633324</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>39323688</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9">
         <v>20803</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9">
         <v>15067</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9">
         <v>121211973</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9">
         <v>4914607463</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9">
         <v>38404117745</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9">
         <v>17365718</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9">
         <v>10330077232</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9">
         <v>7033477</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9">
         <v>201217661645.509</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>2014</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10">
         <v>17331402</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>28449234</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10">
         <v>20058</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10">
         <v>16019</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10">
         <v>230522077</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10">
         <v>5694128857</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10">
         <v>43263274050</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10">
         <v>18271439</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10">
         <v>11494167142</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10">
         <v>7070288</v>
       </c>
-      <c r="L10" s="0" t="n">
-        <v>201080662205.002</v>
+      <c r="L10">
+        <v>201080662205.00201</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>2015</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11">
         <v>14372231</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11">
         <v>19071962</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11">
         <v>20044</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11">
         <v>17417</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11">
         <v>344571836</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11">
         <v>8586273194</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11">
         <v>47994342480</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I11">
         <v>11605091</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11">
         <v>12675369815</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K11">
         <v>7104620</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L11">
         <v>189926516769.25</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>2016</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12">
         <v>14231412</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12">
         <v>14044383</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12">
         <v>18471</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12">
         <v>15989</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12">
         <v>464826243</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12">
         <v>16165825038</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12">
         <v>55746187929</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I12">
         <v>7506784</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12">
         <v>15221087095</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K12">
         <v>7136722</v>
       </c>
-      <c r="L12" s="0" t="n">
-        <v>191639655121.33</v>
+      <c r="L12">
+        <v>191639655121.32999</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
@@ -2587,25 +2927,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col min="1" max="1025" width="11.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>

</xml_diff>